<commit_message>
naadis added to excel and formila fix
</commit_message>
<xml_diff>
--- a/code/Nakshatras.xlsx
+++ b/code/Nakshatras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Param\Documents\IT Solutions\Projects\2023\psAstroMatch\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E5375C-DA63-4DA0-8916-F560532F3143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF86E1B-CD23-4BC9-8800-A081BAE2E851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="7545" windowWidth="17130" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19530" yWindow="6465" windowWidth="17130" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Gana" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="76">
   <si>
     <t>index</t>
   </si>
@@ -253,6 +256,15 @@
   </si>
   <si>
     <t>Bhakut (Rashi)</t>
+  </si>
+  <si>
+    <t>आदि</t>
+  </si>
+  <si>
+    <t>मध्य</t>
+  </si>
+  <si>
+    <t>अंत्य</t>
   </si>
 </sst>
 </file>
@@ -307,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -330,12 +342,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -350,6 +375,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -653,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,9 +692,10 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,8 +708,11 @@
       <c r="D1" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -693,8 +725,11 @@
       <c r="D2" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -707,8 +742,11 @@
       <c r="D3" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -721,8 +759,11 @@
       <c r="D4" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -735,8 +776,11 @@
       <c r="D5" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -749,8 +793,11 @@
       <c r="D6" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -763,8 +810,11 @@
       <c r="D7" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -777,8 +827,11 @@
       <c r="D8" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -791,8 +844,11 @@
       <c r="D9" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -805,8 +861,11 @@
       <c r="D10" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -819,8 +878,11 @@
       <c r="D11" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -833,8 +895,11 @@
       <c r="D12" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -847,8 +912,11 @@
       <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -861,8 +929,11 @@
       <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -875,8 +946,11 @@
       <c r="D15" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -889,8 +963,11 @@
       <c r="D16" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -903,8 +980,11 @@
       <c r="D17" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -917,8 +997,11 @@
       <c r="D18" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -931,8 +1014,11 @@
       <c r="D19" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -945,8 +1031,11 @@
       <c r="D20" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -959,8 +1048,11 @@
       <c r="D21" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -973,8 +1065,11 @@
       <c r="D22" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -987,8 +1082,11 @@
       <c r="D23" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1001,8 +1099,11 @@
       <c r="D24" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -1015,8 +1116,11 @@
       <c r="D25" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -1029,8 +1133,11 @@
       <c r="D26" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1043,8 +1150,11 @@
       <c r="D27" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -1057,9 +1167,13 @@
       <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>